<commit_message>
up to date con main
</commit_message>
<xml_diff>
--- a/RutaCritica/MiMalla.xlsx
+++ b/RutaCritica/MiMalla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\TdR\generador_de_horarios_Practica\RutaCritica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\Downloads\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18B10E-5A49-4058-9A0F-A7C8193C8A0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3721CD64-6167-42FD-8C44-8278655429E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E8A2F0A-3134-4A00-A9B2-0591E032DEE3}"/>
   </bookViews>
@@ -33,7 +33,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+  <si>
+    <t>CBM1000</t>
+  </si>
+  <si>
+    <t>CBM1001</t>
+  </si>
+  <si>
+    <t>CBQ1000</t>
+  </si>
+  <si>
+    <t>CIT1000</t>
+  </si>
+  <si>
+    <t>FIC1000</t>
+  </si>
+  <si>
+    <t>CBM1002</t>
+  </si>
+  <si>
+    <t>CBM1003</t>
+  </si>
+  <si>
+    <t>CBF1000</t>
+  </si>
+  <si>
+    <t>CIT1010</t>
+  </si>
+  <si>
+    <t>CBM1005</t>
+  </si>
+  <si>
+    <t>CBM1006</t>
+  </si>
+  <si>
+    <t>CBF1001</t>
+  </si>
+  <si>
+    <t>CIT2000</t>
+  </si>
+  <si>
+    <t>CIT2100</t>
+  </si>
+  <si>
+    <t>CIT2204</t>
+  </si>
+  <si>
+    <t>CBM2000</t>
+  </si>
+  <si>
+    <t>CBF1002</t>
+  </si>
+  <si>
+    <t>CIT2001</t>
+  </si>
   <si>
     <t>Código</t>
   </si>
@@ -50,17 +104,260 @@
     <t>Abre la/s asignatura/s:</t>
   </si>
   <si>
+    <t>11, 17, 22</t>
+  </si>
+  <si>
+    <t>11, 12, 13, 16, 17</t>
+  </si>
+  <si>
+    <t>14, 15</t>
+  </si>
+  <si>
+    <t>18, 22, 28</t>
+  </si>
+  <si>
+    <t>24, 29, 31</t>
+  </si>
+  <si>
+    <t>29, 30</t>
+  </si>
+  <si>
+    <t>24, 25</t>
+  </si>
+  <si>
+    <t>CFG</t>
+  </si>
+  <si>
+    <t>MECÁNICA</t>
+  </si>
+  <si>
+    <t>CALOR Y ONDAS</t>
+  </si>
+  <si>
+    <t>ELECTRICIDAD Y MAGNETISMO</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA Y GEOMETRÍA</t>
+  </si>
+  <si>
+    <t>CÁLCULO I</t>
+  </si>
+  <si>
+    <t>ÁLGEBRA LINEAL</t>
+  </si>
+  <si>
+    <t>CÁLCULO II</t>
+  </si>
+  <si>
+    <t>ECUACIONES DIFERENCIALES</t>
+  </si>
+  <si>
+    <t>CÁLCULO III</t>
+  </si>
+  <si>
+    <t>MÉTODOS NUMÉRICOS</t>
+  </si>
+  <si>
+    <t>QUÍMICA</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN AVANZADA</t>
+  </si>
+  <si>
+    <t>ESTRUCTURAS DE DATOS</t>
+  </si>
+  <si>
+    <t>DISEÑO Y ANÁLISIS DE ALGORITMOS</t>
+  </si>
+  <si>
+    <t>REDES DE DATOS</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN PARA LA INGENIERÍA</t>
+  </si>
+  <si>
+    <t>INGLÉS I</t>
+  </si>
+  <si>
+    <t>PROBABILIDADES Y ESTADÍSTICAS</t>
+  </si>
+  <si>
+    <t>6, 7</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>7, 8</t>
+  </si>
+  <si>
+    <t>11, 12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Prerreq</t>
   </si>
   <si>
     <t>Equivalencias</t>
+  </si>
+  <si>
+    <t>CIT2006</t>
+  </si>
+  <si>
+    <t>CIG1012</t>
+  </si>
+  <si>
+    <t>CIT2008</t>
+  </si>
+  <si>
+    <t>CIT2114</t>
+  </si>
+  <si>
+    <t>CII2750</t>
+  </si>
+  <si>
+    <t>OPTIMIZACIÓN</t>
+  </si>
+  <si>
+    <t>6, 12</t>
+  </si>
+  <si>
+    <t>CIT2107</t>
+  </si>
+  <si>
+    <t>CII2000</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN  A LA ECONOMÍA</t>
+  </si>
+  <si>
+    <t>CII2100</t>
+  </si>
+  <si>
+    <t>7, 8, 34</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>CIT2106</t>
+  </si>
+  <si>
+    <t>ELECTRÓNICA Y ELECTROTECNIA</t>
+  </si>
+  <si>
+    <t>30, 32</t>
+  </si>
+  <si>
+    <t>CIT2200</t>
+  </si>
+  <si>
+    <t>PROYECTO EN TICS I</t>
+  </si>
+  <si>
+    <t>35, 42</t>
+  </si>
+  <si>
+    <t>15, 19</t>
+  </si>
+  <si>
+    <t>CIT2205</t>
+  </si>
+  <si>
+    <t>CIT2002</t>
+  </si>
+  <si>
+    <t>BASES DE DATOS</t>
+  </si>
+  <si>
+    <t>31, 35</t>
+  </si>
+  <si>
+    <t>CIT2007</t>
+  </si>
+  <si>
+    <t>CIG1013</t>
+  </si>
+  <si>
+    <t>INGLÉS II</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>CIT2202</t>
+  </si>
+  <si>
+    <t>MODELOS ESTOCASTICOS Y SIMULACIÓN</t>
+  </si>
+  <si>
+    <t>15, 16, 22</t>
+  </si>
+  <si>
+    <t>CIT2108</t>
+  </si>
+  <si>
+    <t>CIT2101</t>
+  </si>
+  <si>
+    <t>SEÑALES Y SISTEMAS</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>16, 23</t>
+  </si>
+  <si>
+    <t>CIT2110</t>
+  </si>
+  <si>
+    <t>CIT2003</t>
+  </si>
+  <si>
+    <t>SISTEMAS OPERATIVOS</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>15, 25</t>
+  </si>
+  <si>
+    <t>CIT2010</t>
+  </si>
+  <si>
+    <t>CIT2103</t>
+  </si>
+  <si>
+    <t>SISTEMAS DIGITALES</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>CIT2109</t>
+  </si>
+  <si>
+    <t>CIG1014</t>
+  </si>
+  <si>
+    <t>INGLÉS III</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +374,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,7 +390,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,8 +402,44 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8BDBCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF949A4C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -121,17 +462,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -541,7 +916,7 @@
   <dimension ref="A2:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="A3" sqref="A3:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,172 +924,790 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="16" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="8">
+        <v>9</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="8">
+        <v>38</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8"/>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9"/>
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="18">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10"/>
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>2</v>
+      </c>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11"/>
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="18">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>4</v>
+      </c>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12"/>
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="18">
+        <v>2</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13"/>
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="10">
+        <v>18</v>
+      </c>
+      <c r="E13" s="19">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14"/>
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="19">
+        <v>3</v>
+      </c>
+      <c r="F14" s="10">
+        <v>7</v>
+      </c>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15"/>
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="19">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30"/>
-    </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="10">
+        <v>19</v>
+      </c>
+      <c r="E16" s="19">
+        <v>3</v>
+      </c>
+      <c r="F16" s="10">
+        <v>9</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="19">
+        <v>3</v>
+      </c>
+      <c r="F17" s="10">
+        <v>9</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="20">
+        <v>4</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="20">
+        <v>4</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="11">
+        <v>23</v>
+      </c>
+      <c r="E20" s="20">
+        <v>4</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="20">
+        <v>4</v>
+      </c>
+      <c r="F21" s="11">
+        <v>14</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="20">
+        <v>4</v>
+      </c>
+      <c r="F22" s="11">
+        <v>0</v>
+      </c>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="11">
+        <v>27</v>
+      </c>
+      <c r="E23" s="20">
+        <v>4</v>
+      </c>
+      <c r="F23" s="11">
+        <v>5</v>
+      </c>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="12">
+        <v>29</v>
+      </c>
+      <c r="E24" s="21">
+        <v>5</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="21">
+        <v>5</v>
+      </c>
+      <c r="F25" s="23">
+        <v>18</v>
+      </c>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="21">
+        <v>5</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="21">
+        <v>5</v>
+      </c>
+      <c r="F27" s="12">
+        <v>19</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="21">
+        <v>5</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="21">
+        <v>5</v>
+      </c>
+      <c r="F29" s="12">
+        <v>21</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="22">
+        <v>6</v>
+      </c>
+      <c r="F30" s="13">
+        <v>12</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="22">
+        <v>6</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="22">
+        <v>6</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="22">
+        <v>6</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="22">
+        <v>6</v>
+      </c>
+      <c r="F34" s="13">
+        <v>23</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="22">
+        <v>6</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D36"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D37"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D39"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D40"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D41"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D42"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D43"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D44"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D45"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D46"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D47"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D48"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CFG con menor prioridad
</commit_message>
<xml_diff>
--- a/RutaCritica/MiMalla.xlsx
+++ b/RutaCritica/MiMalla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402E9C7D-D84A-4F6B-9043-255E39ECA1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570B61AF-521C-493B-947C-E7CFD40DA685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="1380" windowWidth="18000" windowHeight="9810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiMalla" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,9 @@
     <t>CÁLCULO I</t>
   </si>
   <si>
+    <t>7, 8, 34</t>
+  </si>
+  <si>
     <t>CBQ1000</t>
   </si>
   <si>
@@ -85,12 +88,21 @@
     <t>PROGRAMACIÓN</t>
   </si>
   <si>
+    <t>FIC1000</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN PARA LA INGENIERÍA</t>
+  </si>
+  <si>
     <t>CBM1003</t>
   </si>
   <si>
     <t>CÁLCULO II</t>
   </si>
   <si>
+    <t>11, 12, 13, 16, 17</t>
+  </si>
+  <si>
     <t>CIT1010</t>
   </si>
   <si>
@@ -124,32 +136,101 @@
     <t>2</t>
   </si>
   <si>
+    <t>CIT2000</t>
+  </si>
+  <si>
+    <t>ESTRUCTURAS DE DATOS</t>
+  </si>
+  <si>
+    <t>CIT2100</t>
+  </si>
+  <si>
+    <t>REDES DE DATOS</t>
+  </si>
+  <si>
+    <t>24, 29, 31</t>
+  </si>
+  <si>
+    <t>CIT2204</t>
+  </si>
+  <si>
+    <t>PROBABILIDADES Y ESTADÍSTICAS</t>
+  </si>
+  <si>
+    <t>29, 30</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>CBM1006</t>
+  </si>
+  <si>
+    <t>CÁLCULO III</t>
+  </si>
+  <si>
+    <t>17, 18, 22</t>
+  </si>
+  <si>
+    <t>CIG1012</t>
+  </si>
+  <si>
+    <t>INGLÉS I</t>
+  </si>
+  <si>
+    <t>CIT2007</t>
+  </si>
+  <si>
+    <t>BASES DE DATOS</t>
+  </si>
+  <si>
+    <t>25, 37, 42</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>CIT2008</t>
+  </si>
+  <si>
+    <t>DESARROLLO WEB Y MÓVIL</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
+    <t>CII1000</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD Y COSTOS</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>CBM1005</t>
+  </si>
+  <si>
+    <t>ECUACIONES DIFERENCIALES</t>
+  </si>
+  <si>
+    <t>17, 18</t>
+  </si>
+  <si>
+    <t>6, 7</t>
+  </si>
+  <si>
     <t>2020</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7, 8, 28</t>
-  </si>
-  <si>
-    <t>11, 12, 16, 39</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>CFG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -202,16 +283,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,14 +327,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFFA7D00"/>
       </patternFill>
     </fill>
   </fills>
@@ -325,7 +392,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -336,15 +403,18 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -445,7 +515,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>419040</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -837,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,15 +923,15 @@
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -881,258 +951,418 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="9">
+        <v>38</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2</v>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>9</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="13">
+        <v>2</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="16">
-        <v>2</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="16">
-        <v>2</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>8</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="16">
-        <v>2</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="16">
-        <v>2</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="E11" s="16">
         <v>2</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>14</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="15">
+        <v>19</v>
+      </c>
+      <c r="E12" s="16">
+        <v>3</v>
+      </c>
+      <c r="F12" s="15">
+        <v>9</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>15</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="16">
+        <v>3</v>
+      </c>
+      <c r="F13" s="15">
+        <v>9</v>
+      </c>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>16</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="19">
+        <v>4</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>12</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="19">
+        <v>3</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>21</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="18">
+        <v>27</v>
+      </c>
+      <c r="E16" s="19">
+        <v>4</v>
+      </c>
+      <c r="F16" s="18">
+        <v>5</v>
+      </c>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>19</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>20</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="19">
+        <v>4</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>28</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>11</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="19">
+        <v>3</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D27"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D32"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
@@ -1143,6 +1373,42 @@
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
fix pert LF was wrong
</commit_message>
<xml_diff>
--- a/RutaCritica/MiMalla.xlsx
+++ b/RutaCritica/MiMalla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Flores\Desktop\practica II 2021\generador_de_horarios_Practica\RutaCritica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5366A89E-A34B-4132-A4B1-415468FF2D9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85C25E9-1A58-4D89-964D-6939379CCD45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MiMalla" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -322,24 +322,6 @@
     <t>DERECHO EN INGENIERÍA</t>
   </si>
   <si>
-    <t>CIT2203</t>
-  </si>
-  <si>
-    <t>GESTIÓN ORGANIZACIONAL</t>
-  </si>
-  <si>
-    <t>CIT2004</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA DE SISTEMAS</t>
-  </si>
-  <si>
-    <t>CIT2105</t>
-  </si>
-  <si>
-    <t>CRIPTOGRAFÍA Y SEGURIDAD EN REDES</t>
-  </si>
-  <si>
     <t>38,21</t>
   </si>
   <si>
@@ -349,28 +331,28 @@
     <t>CFG-2</t>
   </si>
   <si>
-    <t>CIT3310</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 1</t>
-  </si>
-  <si>
-    <t>CIT3410</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 1</t>
-  </si>
-  <si>
-    <t>CIT3411</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL TEL 2</t>
-  </si>
-  <si>
-    <t>CIT3311</t>
-  </si>
-  <si>
-    <t>ELECTIVO PROFESIONAL INF 2</t>
+    <t>CFG1</t>
+  </si>
+  <si>
+    <t>CFG2</t>
+  </si>
+  <si>
+    <t>CFG3</t>
+  </si>
+  <si>
+    <t>CFG-3</t>
+  </si>
+  <si>
+    <t>CIT2102</t>
+  </si>
+  <si>
+    <t>COMUNICACIONES DIGITALES</t>
+  </si>
+  <si>
+    <t>CIT2104</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE COMPUTADORES</t>
   </si>
 </sst>
 </file>
@@ -438,7 +420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,12 +482,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF16B6B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +553,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -587,64 +563,58 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="12" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="12" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="13" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="13" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Entrada" xfId="2" builtinId="20"/>
@@ -1141,20 +1111,20 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A3" sqref="A3:F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1132,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1182,826 +1152,778 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="12">
         <v>0</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="12">
         <v>0</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>9</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="12">
         <v>0</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="16">
         <v>2</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="16">
         <v>4</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="33">
+      <c r="B12" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="16">
         <v>0</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
         <v>11</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="21">
         <v>18</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="20">
         <v>7</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
         <v>14</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="20">
         <v>9</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="21">
         <v>19</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
         <v>15</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="20">
         <v>9</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="25" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="25" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="10">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
         <v>18</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="25">
         <v>23</v>
       </c>
       <c r="F20" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="10">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="24">
         <v>14</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="25" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="10">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="23">
         <v>20</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="35">
+      <c r="B22" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="24">
         <v>0</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="25" t="s">
         <v>47</v>
       </c>
       <c r="F22" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="10">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
         <v>21</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="24">
         <v>5</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="25">
         <v>27</v>
       </c>
       <c r="F23" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
         <v>22</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="29">
         <v>29</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="31">
         <v>18</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="30">
         <v>5</v>
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
         <v>24</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="27">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="28">
         <v>19</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="27">
+        <v>26</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="27">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D29" s="28">
         <v>21</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E29" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F29" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="12">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D30" s="34">
         <v>12</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E30" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F30" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="12">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B31" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D31" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E31" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F31" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D32" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E32" s="35">
         <v>35</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F32" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B33" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D33" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E33" s="35">
         <v>40</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F33" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="12">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D34" s="34">
         <v>23</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E34" s="35">
         <v>37</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F34" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="37">
         <v>33</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B35" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C35" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D35" s="38">
         <v>2</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E35" s="39">
         <v>46</v>
       </c>
-      <c r="F34" s="29">
+      <c r="F35" s="40">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="13">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="37">
         <v>34</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B36" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C36" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D36" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E36" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="29">
+      <c r="F36" s="40">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="13">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="38">
+        <v>30</v>
+      </c>
+      <c r="E37" s="39">
+        <v>41</v>
+      </c>
+      <c r="F37" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="37">
         <v>36</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B38" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C38" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D38" s="38">
         <v>0</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E38" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="29">
+      <c r="F38" s="40">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
-        <v>38</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="40">
-        <v>5</v>
-      </c>
-      <c r="E37" s="22" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="37">
+        <v>37</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="38">
+        <v>32</v>
+      </c>
+      <c r="E39" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F37" s="30">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
-        <v>39</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="40">
-        <v>34</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" s="30">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
-        <v>40</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="40">
-        <v>31</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="30">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="41">
-        <v>43</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" s="44">
-        <v>0</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="43">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="41">
-        <v>44</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="44">
-        <v>0</v>
-      </c>
-      <c r="E41" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="43">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="41">
-        <v>45</v>
-      </c>
-      <c r="B42" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="44">
-        <v>0</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="43">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="41">
-        <v>47</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" s="44">
-        <v>0</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="43">
-        <v>9</v>
-      </c>
+      <c r="F39" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>